<commit_message>
plotted all stations all taxa
</commit_message>
<xml_diff>
--- a/analyses/T7-incubations/unipept/lca/NAAF/MN_phylum_naaf.xlsx
+++ b/analyses/T7-incubations/unipept/lca/NAAF/MN_phylum_naaf.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,6 +14,7 @@
     <sheet name="318" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="417" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="for python" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Sheet7" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -25,9 +26,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="58">
   <si>
-    <t xml:space="preserve">106_phylum</t>
+    <t xml:space="preserve">phylum</t>
   </si>
   <si>
     <t xml:space="preserve">126_Area</t>
@@ -141,19 +142,16 @@
     <t xml:space="preserve">Candidatus Aminicenantes</t>
   </si>
   <si>
-    <t xml:space="preserve">Sample total</t>
+    <t xml:space="preserve">Tubulinea</t>
   </si>
   <si>
-    <t xml:space="preserve">phylum</t>
+    <t xml:space="preserve">Sample total</t>
   </si>
   <si>
     <t xml:space="preserve">Area</t>
   </si>
   <si>
     <t xml:space="preserve">NAAF_num.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tubulinea</t>
   </si>
   <si>
     <t xml:space="preserve">Candidatus Uhrbacteria</t>
@@ -163,6 +161,9 @@
   </si>
   <si>
     <t xml:space="preserve">Candidatus Falkowbacteria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phyla</t>
   </si>
   <si>
     <t xml:space="preserve">Time 0 small</t>
@@ -175,6 +176,30 @@
   </si>
   <si>
     <t xml:space="preserve">Time 24 large</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Candidatus Micrarchaeota</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Candidatus Saccharibacteria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balneolaeota</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thaumarchaeota</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oomycota</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apicomplexa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Haptista</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uroviricota</t>
   </si>
 </sst>
 </file>
@@ -284,10 +309,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R30"/>
+  <dimension ref="A1:R31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q37" activeCellId="0" sqref="Q37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -377,35 +402,35 @@
         <v>37547753.5714286</v>
       </c>
       <c r="K2" s="1" t="n">
-        <f aca="false">B2/B$30*100</f>
+        <f aca="false">B2/B$31*100</f>
         <v>17.5151813995905</v>
       </c>
       <c r="L2" s="1" t="n">
-        <f aca="false">C2/C$30*100</f>
+        <f aca="false">C2/C$31*100</f>
         <v>17.5192788811317</v>
       </c>
       <c r="M2" s="1" t="n">
-        <f aca="false">D2/D$30*100</f>
+        <f aca="false">D2/D$31*100</f>
         <v>27.6059429299848</v>
       </c>
       <c r="N2" s="1" t="n">
-        <f aca="false">E2/E$30*100</f>
+        <f aca="false">E2/E$31*100</f>
         <v>27.6038624269972</v>
       </c>
       <c r="O2" s="1" t="n">
-        <f aca="false">F2/F$30*100</f>
+        <f aca="false">F2/F$31*100</f>
         <v>14.6224340467729</v>
       </c>
       <c r="P2" s="1" t="n">
-        <f aca="false">G2/G$30*100</f>
+        <f aca="false">G2/G$31*100</f>
         <v>14.6182100049843</v>
       </c>
       <c r="Q2" s="1" t="n">
-        <f aca="false">H2/H$30*100</f>
+        <f aca="false">H2/H$31*100</f>
         <v>17.2971897283598</v>
       </c>
       <c r="R2" s="1" t="n">
-        <f aca="false">I2/I$30*100</f>
+        <f aca="false">I2/I$31*100</f>
         <v>17.2976904893594</v>
       </c>
     </row>
@@ -438,35 +463,35 @@
         <v>179331212.5</v>
       </c>
       <c r="K3" s="1" t="n">
-        <f aca="false">B3/B$30*100</f>
+        <f aca="false">B3/B$31*100</f>
         <v>81.7167388937957</v>
       </c>
       <c r="L3" s="1" t="n">
-        <f aca="false">C3/C$30*100</f>
+        <f aca="false">C3/C$31*100</f>
         <v>81.7311297679303</v>
       </c>
       <c r="M3" s="1" t="n">
-        <f aca="false">D3/D$30*100</f>
+        <f aca="false">D3/D$31*100</f>
         <v>72.1122857561404</v>
       </c>
       <c r="N3" s="1" t="n">
-        <f aca="false">E3/E$30*100</f>
+        <f aca="false">E3/E$31*100</f>
         <v>72.1172753215643</v>
       </c>
       <c r="O3" s="1" t="n">
-        <f aca="false">F3/F$30*100</f>
+        <f aca="false">F3/F$31*100</f>
         <v>85.3001602063573</v>
       </c>
       <c r="P3" s="1" t="n">
-        <f aca="false">G3/G$30*100</f>
+        <f aca="false">G3/G$31*100</f>
         <v>85.3070436397842</v>
       </c>
       <c r="Q3" s="1" t="n">
-        <f aca="false">H3/H$30*100</f>
+        <f aca="false">H3/H$31*100</f>
         <v>82.6126833136663</v>
       </c>
       <c r="R3" s="1" t="n">
-        <f aca="false">I3/I$30*100</f>
+        <f aca="false">I3/I$31*100</f>
         <v>82.6152169930871</v>
       </c>
     </row>
@@ -499,35 +524,35 @@
         <v>26400</v>
       </c>
       <c r="K4" s="1" t="n">
-        <f aca="false">B4/B$30*100</f>
+        <f aca="false">B4/B$31*100</f>
         <v>0.0500511018274937</v>
       </c>
       <c r="L4" s="1" t="n">
-        <f aca="false">C4/C$30*100</f>
+        <f aca="false">C4/C$31*100</f>
         <v>0.0460703507228541</v>
       </c>
       <c r="M4" s="1" t="n">
-        <f aca="false">D4/D$30*100</f>
+        <f aca="false">D4/D$31*100</f>
         <v>0.0254432653732578</v>
       </c>
       <c r="N4" s="1" t="n">
-        <f aca="false">E4/E$30*100</f>
+        <f aca="false">E4/E$31*100</f>
         <v>0.0226183918828246</v>
       </c>
       <c r="O4" s="1" t="n">
-        <f aca="false">F4/F$30*100</f>
+        <f aca="false">F4/F$31*100</f>
         <v>0.0107761208509299</v>
       </c>
       <c r="P4" s="1" t="n">
-        <f aca="false">G4/G$30*100</f>
+        <f aca="false">G4/G$31*100</f>
         <v>0.00957914455394675</v>
       </c>
       <c r="Q4" s="1" t="n">
-        <f aca="false">H4/H$30*100</f>
+        <f aca="false">H4/H$31*100</f>
         <v>0.013681424236263</v>
       </c>
       <c r="R4" s="1" t="n">
-        <f aca="false">I4/I$30*100</f>
+        <f aca="false">I4/I$31*100</f>
         <v>0.0121620865560004</v>
       </c>
     </row>
@@ -560,35 +585,35 @@
         <v>0</v>
       </c>
       <c r="K5" s="1" t="n">
-        <f aca="false">B5/B$30*100</f>
+        <f aca="false">B5/B$31*100</f>
         <v>0.0138384573721655</v>
       </c>
       <c r="L5" s="1" t="n">
-        <f aca="false">C5/C$30*100</f>
+        <f aca="false">C5/C$31*100</f>
         <v>0.0138407482001097</v>
       </c>
       <c r="M5" s="1" t="n">
-        <f aca="false">D5/D$30*100</f>
+        <f aca="false">D5/D$31*100</f>
         <v>0.0551484918654368</v>
       </c>
       <c r="N5" s="1" t="n">
-        <f aca="false">E5/E$30*100</f>
+        <f aca="false">E5/E$31*100</f>
         <v>0.0551537491460922</v>
       </c>
       <c r="O5" s="1" t="n">
-        <f aca="false">F5/F$30*100</f>
+        <f aca="false">F5/F$31*100</f>
         <v>0.00538806042546493</v>
       </c>
       <c r="P5" s="1" t="n">
-        <f aca="false">G5/G$30*100</f>
+        <f aca="false">G5/G$31*100</f>
         <v>0.00478957227697338</v>
       </c>
       <c r="Q5" s="1" t="n">
-        <f aca="false">H5/H$30*100</f>
+        <f aca="false">H5/H$31*100</f>
         <v>0</v>
       </c>
       <c r="R5" s="1" t="n">
-        <f aca="false">I5/I$30*100</f>
+        <f aca="false">I5/I$31*100</f>
         <v>0</v>
       </c>
     </row>
@@ -621,35 +646,35 @@
         <v>8800</v>
       </c>
       <c r="K6" s="1" t="n">
-        <f aca="false">B6/B$30*100</f>
+        <f aca="false">B6/B$31*100</f>
         <v>0.0239302581632206</v>
       </c>
       <c r="L6" s="1" t="n">
-        <f aca="false">C6/C$30*100</f>
+        <f aca="false">C6/C$31*100</f>
         <v>0.0212748618621773</v>
       </c>
       <c r="M6" s="1" t="n">
-        <f aca="false">D6/D$30*100</f>
+        <f aca="false">D6/D$31*100</f>
         <v>0</v>
       </c>
       <c r="N6" s="1" t="n">
-        <f aca="false">E6/E$30*100</f>
+        <f aca="false">E6/E$31*100</f>
         <v>0</v>
       </c>
       <c r="O6" s="1" t="n">
-        <f aca="false">F6/F$30*100</f>
+        <f aca="false">F6/F$31*100</f>
         <v>0.0161641812763948</v>
       </c>
       <c r="P6" s="1" t="n">
-        <f aca="false">G6/G$30*100</f>
+        <f aca="false">G6/G$31*100</f>
         <v>0.0143687168309201</v>
       </c>
       <c r="Q6" s="1" t="n">
-        <f aca="false">H6/H$30*100</f>
+        <f aca="false">H6/H$31*100</f>
         <v>0.004560474745421</v>
       </c>
       <c r="R6" s="1" t="n">
-        <f aca="false">I6/I$30*100</f>
+        <f aca="false">I6/I$31*100</f>
         <v>0.00405402885200013</v>
       </c>
     </row>
@@ -682,35 +707,35 @@
         <v>8800</v>
       </c>
       <c r="K7" s="1" t="n">
-        <f aca="false">B7/B$30*100</f>
+        <f aca="false">B7/B$31*100</f>
         <v>0.035895387244831</v>
       </c>
       <c r="L7" s="1" t="n">
-        <f aca="false">C7/C$30*100</f>
+        <f aca="false">C7/C$31*100</f>
         <v>0.0319122927932659</v>
       </c>
       <c r="M7" s="1" t="n">
-        <f aca="false">D7/D$30*100</f>
+        <f aca="false">D7/D$31*100</f>
         <v>0.0150881990365826</v>
       </c>
       <c r="N7" s="1" t="n">
-        <f aca="false">E7/E$30*100</f>
+        <f aca="false">E7/E$31*100</f>
         <v>0.01509116731143</v>
       </c>
       <c r="O7" s="1" t="n">
-        <f aca="false">F7/F$30*100</f>
+        <f aca="false">F7/F$31*100</f>
         <v>0</v>
       </c>
       <c r="P7" s="1" t="n">
-        <f aca="false">G7/G$30*100</f>
+        <f aca="false">G7/G$31*100</f>
         <v>0</v>
       </c>
       <c r="Q7" s="1" t="n">
-        <f aca="false">H7/H$30*100</f>
+        <f aca="false">H7/H$31*100</f>
         <v>0.004560474745421</v>
       </c>
       <c r="R7" s="1" t="n">
-        <f aca="false">I7/I$30*100</f>
+        <f aca="false">I7/I$31*100</f>
         <v>0.00405402885200013</v>
       </c>
     </row>
@@ -743,35 +768,35 @@
         <v>136250</v>
       </c>
       <c r="K8" s="1" t="n">
-        <f aca="false">B8/B$30*100</f>
+        <f aca="false">B8/B$31*100</f>
         <v>0</v>
       </c>
       <c r="L8" s="1" t="n">
-        <f aca="false">C8/C$30*100</f>
+        <f aca="false">C8/C$31*100</f>
         <v>0</v>
       </c>
       <c r="M8" s="1" t="n">
-        <f aca="false">D8/D$30*100</f>
+        <f aca="false">D8/D$31*100</f>
         <v>0.0882375869846989</v>
       </c>
       <c r="N8" s="1" t="n">
-        <f aca="false">E8/E$30*100</f>
+        <f aca="false">E8/E$31*100</f>
         <v>0.0882459986337475</v>
       </c>
       <c r="O8" s="1" t="n">
-        <f aca="false">F8/F$30*100</f>
+        <f aca="false">F8/F$31*100</f>
         <v>0</v>
       </c>
       <c r="P8" s="1" t="n">
-        <f aca="false">G8/G$30*100</f>
+        <f aca="false">G8/G$31*100</f>
         <v>0</v>
       </c>
       <c r="Q8" s="1" t="n">
-        <f aca="false">H8/H$30*100</f>
+        <f aca="false">H8/H$31*100</f>
         <v>0.0627641095013748</v>
       </c>
       <c r="R8" s="1" t="n">
-        <f aca="false">I8/I$30*100</f>
+        <f aca="false">I8/I$31*100</f>
         <v>0.0627683444414793</v>
       </c>
     </row>
@@ -804,35 +829,35 @@
         <v>0</v>
       </c>
       <c r="K9" s="1" t="n">
-        <f aca="false">B9/B$30*100</f>
+        <f aca="false">B9/B$31*100</f>
         <v>0</v>
       </c>
       <c r="L9" s="1" t="n">
-        <f aca="false">C9/C$30*100</f>
+        <f aca="false">C9/C$31*100</f>
         <v>0</v>
       </c>
       <c r="M9" s="1" t="n">
-        <f aca="false">D9/D$30*100</f>
+        <f aca="false">D9/D$31*100</f>
         <v>0</v>
       </c>
       <c r="N9" s="1" t="n">
-        <f aca="false">E9/E$30*100</f>
+        <f aca="false">E9/E$31*100</f>
         <v>0</v>
       </c>
       <c r="O9" s="1" t="n">
-        <f aca="false">F9/F$30*100</f>
+        <f aca="false">F9/F$31*100</f>
         <v>0</v>
       </c>
       <c r="P9" s="1" t="n">
-        <f aca="false">G9/G$30*100</f>
+        <f aca="false">G9/G$31*100</f>
         <v>0</v>
       </c>
       <c r="Q9" s="1" t="n">
-        <f aca="false">H9/H$30*100</f>
+        <f aca="false">H9/H$31*100</f>
         <v>0</v>
       </c>
       <c r="R9" s="1" t="n">
-        <f aca="false">I9/I$30*100</f>
+        <f aca="false">I9/I$31*100</f>
         <v>0</v>
       </c>
     </row>
@@ -865,35 +890,35 @@
         <v>0</v>
       </c>
       <c r="K10" s="1" t="n">
-        <f aca="false">B10/B$30*100</f>
+        <f aca="false">B10/B$31*100</f>
         <v>0</v>
       </c>
       <c r="L10" s="1" t="n">
-        <f aca="false">C10/C$30*100</f>
+        <f aca="false">C10/C$31*100</f>
         <v>0</v>
       </c>
       <c r="M10" s="1" t="n">
-        <f aca="false">D10/D$30*100</f>
+        <f aca="false">D10/D$31*100</f>
         <v>0.00848108845775261</v>
       </c>
       <c r="N10" s="1" t="n">
-        <f aca="false">E10/E$30*100</f>
+        <f aca="false">E10/E$31*100</f>
         <v>0.00753946396094154</v>
       </c>
       <c r="O10" s="1" t="n">
-        <f aca="false">F10/F$30*100</f>
+        <f aca="false">F10/F$31*100</f>
         <v>0</v>
       </c>
       <c r="P10" s="1" t="n">
-        <f aca="false">G10/G$30*100</f>
+        <f aca="false">G10/G$31*100</f>
         <v>0</v>
       </c>
       <c r="Q10" s="1" t="n">
-        <f aca="false">H10/H$30*100</f>
+        <f aca="false">H10/H$31*100</f>
         <v>0</v>
       </c>
       <c r="R10" s="1" t="n">
-        <f aca="false">I10/I$30*100</f>
+        <f aca="false">I10/I$31*100</f>
         <v>0</v>
       </c>
     </row>
@@ -926,35 +951,35 @@
         <v>8800</v>
       </c>
       <c r="K11" s="1" t="n">
-        <f aca="false">B11/B$30*100</f>
+        <f aca="false">B11/B$31*100</f>
         <v>0.035895387244831</v>
       </c>
       <c r="L11" s="1" t="n">
-        <f aca="false">C11/C$30*100</f>
+        <f aca="false">C11/C$31*100</f>
         <v>0.0319122927932659</v>
       </c>
       <c r="M11" s="1" t="n">
-        <f aca="false">D11/D$30*100</f>
+        <f aca="false">D11/D$31*100</f>
         <v>0.0124217962260013</v>
       </c>
       <c r="N11" s="1" t="n">
-        <f aca="false">E11/E$30*100</f>
+        <f aca="false">E11/E$31*100</f>
         <v>0.0141976918745003</v>
       </c>
       <c r="O11" s="1" t="n">
-        <f aca="false">F11/F$30*100</f>
+        <f aca="false">F11/F$31*100</f>
         <v>0.0225454952651399</v>
       </c>
       <c r="P11" s="1" t="n">
-        <f aca="false">G11/G$30*100</f>
+        <f aca="false">G11/G$31*100</f>
         <v>0.0252722506887269</v>
       </c>
       <c r="Q11" s="1" t="n">
-        <f aca="false">H11/H$30*100</f>
+        <f aca="false">H11/H$31*100</f>
         <v>0.004560474745421</v>
       </c>
       <c r="R11" s="1" t="n">
-        <f aca="false">I11/I$30*100</f>
+        <f aca="false">I11/I$31*100</f>
         <v>0.00405402885200013</v>
       </c>
     </row>
@@ -987,35 +1012,35 @@
         <v>0</v>
       </c>
       <c r="K12" s="1" t="n">
-        <f aca="false">B12/B$30*100</f>
+        <f aca="false">B12/B$31*100</f>
         <v>0</v>
       </c>
       <c r="L12" s="1" t="n">
-        <f aca="false">C12/C$30*100</f>
+        <f aca="false">C12/C$31*100</f>
         <v>0</v>
       </c>
       <c r="M12" s="1" t="n">
-        <f aca="false">D12/D$30*100</f>
+        <f aca="false">D12/D$31*100</f>
         <v>0</v>
       </c>
       <c r="N12" s="1" t="n">
-        <f aca="false">E12/E$30*100</f>
+        <f aca="false">E12/E$31*100</f>
         <v>0</v>
       </c>
       <c r="O12" s="1" t="n">
-        <f aca="false">F12/F$30*100</f>
+        <f aca="false">F12/F$31*100</f>
         <v>0</v>
       </c>
       <c r="P12" s="1" t="n">
-        <f aca="false">G12/G$30*100</f>
+        <f aca="false">G12/G$31*100</f>
         <v>0</v>
       </c>
       <c r="Q12" s="1" t="n">
-        <f aca="false">H12/H$30*100</f>
+        <f aca="false">H12/H$31*100</f>
         <v>0</v>
       </c>
       <c r="R12" s="1" t="n">
-        <f aca="false">I12/I$30*100</f>
+        <f aca="false">I12/I$31*100</f>
         <v>0</v>
       </c>
     </row>
@@ -1048,35 +1073,35 @@
         <v>0</v>
       </c>
       <c r="K13" s="1" t="n">
-        <f aca="false">B13/B$30*100</f>
+        <f aca="false">B13/B$31*100</f>
         <v>0</v>
       </c>
       <c r="L13" s="1" t="n">
-        <f aca="false">C13/C$30*100</f>
+        <f aca="false">C13/C$31*100</f>
         <v>0</v>
       </c>
       <c r="M13" s="1" t="n">
-        <f aca="false">D13/D$30*100</f>
+        <f aca="false">D13/D$31*100</f>
         <v>0</v>
       </c>
       <c r="N13" s="1" t="n">
-        <f aca="false">E13/E$30*100</f>
+        <f aca="false">E13/E$31*100</f>
         <v>0</v>
       </c>
       <c r="O13" s="1" t="n">
-        <f aca="false">F13/F$30*100</f>
+        <f aca="false">F13/F$31*100</f>
         <v>0.00538806042546493</v>
       </c>
       <c r="P13" s="1" t="n">
-        <f aca="false">G13/G$30*100</f>
+        <f aca="false">G13/G$31*100</f>
         <v>0.00478957227697338</v>
       </c>
       <c r="Q13" s="1" t="n">
-        <f aca="false">H13/H$30*100</f>
+        <f aca="false">H13/H$31*100</f>
         <v>0</v>
       </c>
       <c r="R13" s="1" t="n">
-        <f aca="false">I13/I$30*100</f>
+        <f aca="false">I13/I$31*100</f>
         <v>0</v>
       </c>
     </row>
@@ -1109,35 +1134,35 @@
         <v>0</v>
       </c>
       <c r="K14" s="1" t="n">
-        <f aca="false">B14/B$30*100</f>
+        <f aca="false">B14/B$31*100</f>
         <v>0.0119651290816103</v>
       </c>
       <c r="L14" s="1" t="n">
-        <f aca="false">C14/C$30*100</f>
+        <f aca="false">C14/C$31*100</f>
         <v>0.0106374309310886</v>
       </c>
       <c r="M14" s="1" t="n">
-        <f aca="false">D14/D$30*100</f>
+        <f aca="false">D14/D$31*100</f>
         <v>0</v>
       </c>
       <c r="N14" s="1" t="n">
-        <f aca="false">E14/E$30*100</f>
+        <f aca="false">E14/E$31*100</f>
         <v>0</v>
       </c>
       <c r="O14" s="1" t="n">
-        <f aca="false">F14/F$30*100</f>
+        <f aca="false">F14/F$31*100</f>
         <v>0.00126537782719252</v>
       </c>
       <c r="P14" s="1" t="n">
-        <f aca="false">G14/G$30*100</f>
+        <f aca="false">G14/G$31*100</f>
         <v>0.00126542676635944</v>
       </c>
       <c r="Q14" s="1" t="n">
-        <f aca="false">H14/H$30*100</f>
+        <f aca="false">H14/H$31*100</f>
         <v>0</v>
       </c>
       <c r="R14" s="1" t="n">
-        <f aca="false">I14/I$30*100</f>
+        <f aca="false">I14/I$31*100</f>
         <v>0</v>
       </c>
     </row>
@@ -1170,35 +1195,35 @@
         <v>0</v>
       </c>
       <c r="K15" s="1" t="n">
-        <f aca="false">B15/B$30*100</f>
+        <f aca="false">B15/B$31*100</f>
         <v>0.0119651290816103</v>
       </c>
       <c r="L15" s="1" t="n">
-        <f aca="false">C15/C$30*100</f>
+        <f aca="false">C15/C$31*100</f>
         <v>0.0106374309310886</v>
       </c>
       <c r="M15" s="1" t="n">
-        <f aca="false">D15/D$30*100</f>
+        <f aca="false">D15/D$31*100</f>
         <v>0.00848108845775261</v>
       </c>
       <c r="N15" s="1" t="n">
-        <f aca="false">E15/E$30*100</f>
+        <f aca="false">E15/E$31*100</f>
         <v>0.00753946396094154</v>
       </c>
       <c r="O15" s="1" t="n">
-        <f aca="false">F15/F$30*100</f>
+        <f aca="false">F15/F$31*100</f>
         <v>0.00538806042546493</v>
       </c>
       <c r="P15" s="1" t="n">
-        <f aca="false">G15/G$30*100</f>
+        <f aca="false">G15/G$31*100</f>
         <v>0.00478957227697338</v>
       </c>
       <c r="Q15" s="1" t="n">
-        <f aca="false">H15/H$30*100</f>
+        <f aca="false">H15/H$31*100</f>
         <v>0</v>
       </c>
       <c r="R15" s="1" t="n">
-        <f aca="false">I15/I$30*100</f>
+        <f aca="false">I15/I$31*100</f>
         <v>0</v>
       </c>
     </row>
@@ -1231,35 +1256,35 @@
         <v>0</v>
       </c>
       <c r="K16" s="1" t="n">
-        <f aca="false">B16/B$30*100</f>
+        <f aca="false">B16/B$31*100</f>
         <v>0</v>
       </c>
       <c r="L16" s="1" t="n">
-        <f aca="false">C16/C$30*100</f>
+        <f aca="false">C16/C$31*100</f>
         <v>0</v>
       </c>
       <c r="M16" s="1" t="n">
-        <f aca="false">D16/D$30*100</f>
+        <f aca="false">D16/D$31*100</f>
         <v>0</v>
       </c>
       <c r="N16" s="1" t="n">
-        <f aca="false">E16/E$30*100</f>
+        <f aca="false">E16/E$31*100</f>
         <v>0</v>
       </c>
       <c r="O16" s="1" t="n">
-        <f aca="false">F16/F$30*100</f>
+        <f aca="false">F16/F$31*100</f>
         <v>0</v>
       </c>
       <c r="P16" s="1" t="n">
-        <f aca="false">G16/G$30*100</f>
+        <f aca="false">G16/G$31*100</f>
         <v>0</v>
       </c>
       <c r="Q16" s="1" t="n">
-        <f aca="false">H16/H$30*100</f>
+        <f aca="false">H16/H$31*100</f>
         <v>0</v>
       </c>
       <c r="R16" s="1" t="n">
-        <f aca="false">I16/I$30*100</f>
+        <f aca="false">I16/I$31*100</f>
         <v>0</v>
       </c>
     </row>
@@ -1292,35 +1317,35 @@
         <v>0</v>
       </c>
       <c r="K17" s="1" t="n">
-        <f aca="false">B17/B$30*100</f>
+        <f aca="false">B17/B$31*100</f>
         <v>0</v>
       </c>
       <c r="L17" s="1" t="n">
-        <f aca="false">C17/C$30*100</f>
+        <f aca="false">C17/C$31*100</f>
         <v>0</v>
       </c>
       <c r="M17" s="1" t="n">
-        <f aca="false">D17/D$30*100</f>
+        <f aca="false">D17/D$31*100</f>
         <v>0</v>
       </c>
       <c r="N17" s="1" t="n">
-        <f aca="false">E17/E$30*100</f>
+        <f aca="false">E17/E$31*100</f>
         <v>0</v>
       </c>
       <c r="O17" s="1" t="n">
-        <f aca="false">F17/F$30*100</f>
+        <f aca="false">F17/F$31*100</f>
         <v>0</v>
       </c>
       <c r="P17" s="1" t="n">
-        <f aca="false">G17/G$30*100</f>
+        <f aca="false">G17/G$31*100</f>
         <v>0</v>
       </c>
       <c r="Q17" s="1" t="n">
-        <f aca="false">H17/H$30*100</f>
+        <f aca="false">H17/H$31*100</f>
         <v>0</v>
       </c>
       <c r="R17" s="1" t="n">
-        <f aca="false">I17/I$30*100</f>
+        <f aca="false">I17/I$31*100</f>
         <v>0</v>
       </c>
     </row>
@@ -1353,35 +1378,35 @@
         <v>0</v>
       </c>
       <c r="K18" s="1" t="n">
-        <f aca="false">B18/B$30*100</f>
+        <f aca="false">B18/B$31*100</f>
         <v>0.481928810231527</v>
       </c>
       <c r="L18" s="1" t="n">
-        <f aca="false">C18/C$30*100</f>
+        <f aca="false">C18/C$31*100</f>
         <v>0.482008589064954</v>
       </c>
       <c r="M18" s="1" t="n">
-        <f aca="false">D18/D$30*100</f>
+        <f aca="false">D18/D$31*100</f>
         <v>0.068469797473321</v>
       </c>
       <c r="N18" s="1" t="n">
-        <f aca="false">E18/E$30*100</f>
+        <f aca="false">E18/E$31*100</f>
         <v>0.0684763246679832</v>
       </c>
       <c r="O18" s="1" t="n">
-        <f aca="false">F18/F$30*100</f>
+        <f aca="false">F18/F$31*100</f>
         <v>0.00510232994835694</v>
       </c>
       <c r="P18" s="1" t="n">
-        <f aca="false">G18/G$30*100</f>
+        <f aca="false">G18/G$31*100</f>
         <v>0.00510252728370743</v>
       </c>
       <c r="Q18" s="1" t="n">
-        <f aca="false">H18/H$30*100</f>
+        <f aca="false">H18/H$31*100</f>
         <v>0</v>
       </c>
       <c r="R18" s="1" t="n">
-        <f aca="false">I18/I$30*100</f>
+        <f aca="false">I18/I$31*100</f>
         <v>0</v>
       </c>
     </row>
@@ -1414,35 +1439,35 @@
         <v>0</v>
       </c>
       <c r="K19" s="1" t="n">
-        <f aca="false">B19/B$30*100</f>
+        <f aca="false">B19/B$31*100</f>
         <v>0</v>
       </c>
       <c r="L19" s="1" t="n">
-        <f aca="false">C19/C$30*100</f>
+        <f aca="false">C19/C$31*100</f>
         <v>0</v>
       </c>
       <c r="M19" s="1" t="n">
-        <f aca="false">D19/D$30*100</f>
+        <f aca="false">D19/D$31*100</f>
         <v>0</v>
       </c>
       <c r="N19" s="1" t="n">
-        <f aca="false">E19/E$30*100</f>
+        <f aca="false">E19/E$31*100</f>
         <v>0</v>
       </c>
       <c r="O19" s="1" t="n">
-        <f aca="false">F19/F$30*100</f>
+        <f aca="false">F19/F$31*100</f>
         <v>0</v>
       </c>
       <c r="P19" s="1" t="n">
-        <f aca="false">G19/G$30*100</f>
+        <f aca="false">G19/G$31*100</f>
         <v>0</v>
       </c>
       <c r="Q19" s="1" t="n">
-        <f aca="false">H19/H$30*100</f>
+        <f aca="false">H19/H$31*100</f>
         <v>0</v>
       </c>
       <c r="R19" s="1" t="n">
-        <f aca="false">I19/I$30*100</f>
+        <f aca="false">I19/I$31*100</f>
         <v>0</v>
       </c>
     </row>
@@ -1475,35 +1500,35 @@
         <v>0</v>
       </c>
       <c r="K20" s="1" t="n">
-        <f aca="false">B20/B$30*100</f>
+        <f aca="false">B20/B$31*100</f>
         <v>0.102610046366537</v>
       </c>
       <c r="L20" s="1" t="n">
-        <f aca="false">C20/C$30*100</f>
+        <f aca="false">C20/C$31*100</f>
         <v>0.101297353639231</v>
       </c>
       <c r="M20" s="1" t="n">
-        <f aca="false">D20/D$30*100</f>
+        <f aca="false">D20/D$31*100</f>
         <v>0</v>
       </c>
       <c r="N20" s="1" t="n">
-        <f aca="false">E20/E$30*100</f>
+        <f aca="false">E20/E$31*100</f>
         <v>0</v>
       </c>
       <c r="O20" s="1" t="n">
-        <f aca="false">F20/F$30*100</f>
+        <f aca="false">F20/F$31*100</f>
         <v>0.00538806042546493</v>
       </c>
       <c r="P20" s="1" t="n">
-        <f aca="false">G20/G$30*100</f>
+        <f aca="false">G20/G$31*100</f>
         <v>0.00478957227697338</v>
       </c>
       <c r="Q20" s="1" t="n">
-        <f aca="false">H20/H$30*100</f>
+        <f aca="false">H20/H$31*100</f>
         <v>0</v>
       </c>
       <c r="R20" s="1" t="n">
-        <f aca="false">I20/I$30*100</f>
+        <f aca="false">I20/I$31*100</f>
         <v>0</v>
       </c>
     </row>
@@ -1536,35 +1561,35 @@
         <v>0</v>
       </c>
       <c r="K21" s="1" t="n">
-        <f aca="false">B21/B$30*100</f>
+        <f aca="false">B21/B$31*100</f>
         <v>0</v>
       </c>
       <c r="L21" s="1" t="n">
-        <f aca="false">C21/C$30*100</f>
+        <f aca="false">C21/C$31*100</f>
         <v>0</v>
       </c>
       <c r="M21" s="1" t="n">
-        <f aca="false">D21/D$30*100</f>
+        <f aca="false">D21/D$31*100</f>
         <v>0</v>
       </c>
       <c r="N21" s="1" t="n">
-        <f aca="false">E21/E$30*100</f>
+        <f aca="false">E21/E$31*100</f>
         <v>0</v>
       </c>
       <c r="O21" s="1" t="n">
-        <f aca="false">F21/F$30*100</f>
+        <f aca="false">F21/F$31*100</f>
         <v>0</v>
       </c>
       <c r="P21" s="1" t="n">
-        <f aca="false">G21/G$30*100</f>
+        <f aca="false">G21/G$31*100</f>
         <v>0</v>
       </c>
       <c r="Q21" s="1" t="n">
-        <f aca="false">H21/H$30*100</f>
+        <f aca="false">H21/H$31*100</f>
         <v>0</v>
       </c>
       <c r="R21" s="1" t="n">
-        <f aca="false">I21/I$30*100</f>
+        <f aca="false">I21/I$31*100</f>
         <v>0</v>
       </c>
     </row>
@@ -1597,35 +1622,35 @@
         <v>0</v>
       </c>
       <c r="K22" s="1" t="n">
-        <f aca="false">B22/B$30*100</f>
+        <f aca="false">B22/B$31*100</f>
         <v>0</v>
       </c>
       <c r="L22" s="1" t="n">
-        <f aca="false">C22/C$30*100</f>
+        <f aca="false">C22/C$31*100</f>
         <v>0</v>
       </c>
       <c r="M22" s="1" t="n">
-        <f aca="false">D22/D$30*100</f>
+        <f aca="false">D22/D$31*100</f>
         <v>0</v>
       </c>
       <c r="N22" s="1" t="n">
-        <f aca="false">E22/E$30*100</f>
+        <f aca="false">E22/E$31*100</f>
         <v>0</v>
       </c>
       <c r="O22" s="1" t="n">
-        <f aca="false">F22/F$30*100</f>
+        <f aca="false">F22/F$31*100</f>
         <v>0</v>
       </c>
       <c r="P22" s="1" t="n">
-        <f aca="false">G22/G$30*100</f>
+        <f aca="false">G22/G$31*100</f>
         <v>0</v>
       </c>
       <c r="Q22" s="1" t="n">
-        <f aca="false">H22/H$30*100</f>
+        <f aca="false">H22/H$31*100</f>
         <v>0</v>
       </c>
       <c r="R22" s="1" t="n">
-        <f aca="false">I22/I$30*100</f>
+        <f aca="false">I22/I$31*100</f>
         <v>0</v>
       </c>
     </row>
@@ -1658,35 +1683,35 @@
         <v>0</v>
       </c>
       <c r="K23" s="1" t="n">
-        <f aca="false">B23/B$30*100</f>
+        <f aca="false">B23/B$31*100</f>
         <v>0</v>
       </c>
       <c r="L23" s="1" t="n">
-        <f aca="false">C23/C$30*100</f>
+        <f aca="false">C23/C$31*100</f>
         <v>0</v>
       </c>
       <c r="M23" s="1" t="n">
-        <f aca="false">D23/D$30*100</f>
+        <f aca="false">D23/D$31*100</f>
         <v>0</v>
       </c>
       <c r="N23" s="1" t="n">
-        <f aca="false">E23/E$30*100</f>
+        <f aca="false">E23/E$31*100</f>
         <v>0</v>
       </c>
       <c r="O23" s="1" t="n">
-        <f aca="false">F23/F$30*100</f>
+        <f aca="false">F23/F$31*100</f>
         <v>0</v>
       </c>
       <c r="P23" s="1" t="n">
-        <f aca="false">G23/G$30*100</f>
+        <f aca="false">G23/G$31*100</f>
         <v>0</v>
       </c>
       <c r="Q23" s="1" t="n">
-        <f aca="false">H23/H$30*100</f>
+        <f aca="false">H23/H$31*100</f>
         <v>0</v>
       </c>
       <c r="R23" s="1" t="n">
-        <f aca="false">I23/I$30*100</f>
+        <f aca="false">I23/I$31*100</f>
         <v>0</v>
       </c>
     </row>
@@ -1719,35 +1744,35 @@
         <v>0</v>
       </c>
       <c r="K24" s="1" t="n">
-        <f aca="false">B24/B$30*100</f>
+        <f aca="false">B24/B$31*100</f>
         <v>0.0119651290816103</v>
       </c>
       <c r="L24" s="1" t="n">
-        <f aca="false">C24/C$30*100</f>
+        <f aca="false">C24/C$31*100</f>
         <v>0.0106374309310886</v>
       </c>
       <c r="M24" s="1" t="n">
-        <f aca="false">D24/D$30*100</f>
+        <f aca="false">D24/D$31*100</f>
         <v>0</v>
       </c>
       <c r="N24" s="1" t="n">
-        <f aca="false">E24/E$30*100</f>
+        <f aca="false">E24/E$31*100</f>
         <v>0</v>
       </c>
       <c r="O24" s="1" t="n">
-        <f aca="false">F24/F$30*100</f>
+        <f aca="false">F24/F$31*100</f>
         <v>0.00538806042546493</v>
       </c>
       <c r="P24" s="1" t="n">
-        <f aca="false">G24/G$30*100</f>
+        <f aca="false">G24/G$31*100</f>
         <v>0.00478957227697338</v>
       </c>
       <c r="Q24" s="1" t="n">
-        <f aca="false">H24/H$30*100</f>
+        <f aca="false">H24/H$31*100</f>
         <v>0</v>
       </c>
       <c r="R24" s="1" t="n">
-        <f aca="false">I24/I$30*100</f>
+        <f aca="false">I24/I$31*100</f>
         <v>0</v>
       </c>
     </row>
@@ -1780,35 +1805,35 @@
         <v>0</v>
       </c>
       <c r="K25" s="1" t="n">
-        <f aca="false">B25/B$30*100</f>
+        <f aca="false">B25/B$31*100</f>
         <v>0.0119651290816103</v>
       </c>
       <c r="L25" s="1" t="n">
-        <f aca="false">C25/C$30*100</f>
+        <f aca="false">C25/C$31*100</f>
         <v>0.0106374309310886</v>
       </c>
       <c r="M25" s="1" t="n">
-        <f aca="false">D25/D$30*100</f>
+        <f aca="false">D25/D$31*100</f>
         <v>0</v>
       </c>
       <c r="N25" s="1" t="n">
-        <f aca="false">E25/E$30*100</f>
+        <f aca="false">E25/E$31*100</f>
         <v>0</v>
       </c>
       <c r="O25" s="1" t="n">
-        <f aca="false">F25/F$30*100</f>
+        <f aca="false">F25/F$31*100</f>
         <v>0</v>
       </c>
       <c r="P25" s="1" t="n">
-        <f aca="false">G25/G$30*100</f>
+        <f aca="false">G25/G$31*100</f>
         <v>0</v>
       </c>
       <c r="Q25" s="1" t="n">
-        <f aca="false">H25/H$30*100</f>
+        <f aca="false">H25/H$31*100</f>
         <v>0</v>
       </c>
       <c r="R25" s="1" t="n">
-        <f aca="false">I25/I$30*100</f>
+        <f aca="false">I25/I$31*100</f>
         <v>0</v>
       </c>
     </row>
@@ -1841,35 +1866,35 @@
         <v>91250</v>
       </c>
       <c r="K26" s="1" t="n">
-        <f aca="false">B26/B$30*100</f>
+        <f aca="false">B26/B$31*100</f>
         <v>0</v>
       </c>
       <c r="L26" s="1" t="n">
-        <f aca="false">C26/C$30*100</f>
+        <f aca="false">C26/C$31*100</f>
         <v>0</v>
       </c>
       <c r="M26" s="1" t="n">
-        <f aca="false">D26/D$30*100</f>
+        <f aca="false">D26/D$31*100</f>
         <v>0</v>
       </c>
       <c r="N26" s="1" t="n">
-        <f aca="false">E26/E$30*100</f>
+        <f aca="false">E26/E$31*100</f>
         <v>0</v>
       </c>
       <c r="O26" s="1" t="n">
-        <f aca="false">F26/F$30*100</f>
+        <f aca="false">F26/F$31*100</f>
         <v>0</v>
       </c>
       <c r="P26" s="1" t="n">
-        <f aca="false">G26/G$30*100</f>
+        <f aca="false">G26/G$31*100</f>
         <v>0</v>
       </c>
       <c r="Q26" s="1" t="n">
-        <f aca="false">H26/H$30*100</f>
+        <f aca="false">H26/H$31*100</f>
         <v>0.0420346788403703</v>
       </c>
       <c r="R26" s="1" t="n">
-        <f aca="false">I26/I$30*100</f>
+        <f aca="false">I26/I$31*100</f>
         <v>0.0420375150846605</v>
       </c>
     </row>
@@ -1902,35 +1927,35 @@
         <v>0</v>
       </c>
       <c r="K27" s="1" t="n">
-        <f aca="false">B27/B$30*100</f>
+        <f aca="false">B27/B$31*100</f>
         <v>0</v>
       </c>
       <c r="L27" s="1" t="n">
-        <f aca="false">C27/C$30*100</f>
+        <f aca="false">C27/C$31*100</f>
         <v>0</v>
       </c>
       <c r="M27" s="1" t="n">
-        <f aca="false">D27/D$30*100</f>
+        <f aca="false">D27/D$31*100</f>
         <v>0</v>
       </c>
       <c r="N27" s="1" t="n">
-        <f aca="false">E27/E$30*100</f>
+        <f aca="false">E27/E$31*100</f>
         <v>0</v>
       </c>
       <c r="O27" s="1" t="n">
-        <f aca="false">F27/F$30*100</f>
+        <f aca="false">F27/F$31*100</f>
         <v>0.00538806042546493</v>
       </c>
       <c r="P27" s="1" t="n">
-        <f aca="false">G27/G$30*100</f>
+        <f aca="false">G27/G$31*100</f>
         <v>0.00478957227697338</v>
       </c>
       <c r="Q27" s="1" t="n">
-        <f aca="false">H27/H$30*100</f>
+        <f aca="false">H27/H$31*100</f>
         <v>0</v>
       </c>
       <c r="R27" s="1" t="n">
-        <f aca="false">I27/I$30*100</f>
+        <f aca="false">I27/I$31*100</f>
         <v>0</v>
       </c>
     </row>
@@ -1963,35 +1988,35 @@
         <v>0</v>
       </c>
       <c r="K28" s="1" t="n">
-        <f aca="false">B28/B$30*100</f>
+        <f aca="false">B28/B$31*100</f>
         <v>0</v>
       </c>
       <c r="L28" s="1" t="n">
-        <f aca="false">C28/C$30*100</f>
+        <f aca="false">C28/C$31*100</f>
         <v>0</v>
       </c>
       <c r="M28" s="1" t="n">
-        <f aca="false">D28/D$30*100</f>
+        <f aca="false">D28/D$31*100</f>
         <v>0.00848108845775261</v>
       </c>
       <c r="N28" s="1" t="n">
-        <f aca="false">E28/E$30*100</f>
+        <f aca="false">E28/E$31*100</f>
         <v>0.00753946396094154</v>
       </c>
       <c r="O28" s="1" t="n">
-        <f aca="false">F28/F$30*100</f>
+        <f aca="false">F28/F$31*100</f>
         <v>0</v>
       </c>
       <c r="P28" s="1" t="n">
-        <f aca="false">G28/G$30*100</f>
+        <f aca="false">G28/G$31*100</f>
         <v>0</v>
       </c>
       <c r="Q28" s="1" t="n">
-        <f aca="false">H28/H$30*100</f>
+        <f aca="false">H28/H$31*100</f>
         <v>0</v>
       </c>
       <c r="R28" s="1" t="n">
-        <f aca="false">I28/I$30*100</f>
+        <f aca="false">I28/I$31*100</f>
         <v>0</v>
       </c>
     </row>
@@ -2024,35 +2049,35 @@
         <v>0</v>
       </c>
       <c r="K29" s="1" t="n">
-        <f aca="false">B29/B$30*100</f>
+        <f aca="false">B29/B$31*100</f>
         <v>0</v>
       </c>
       <c r="L29" s="1" t="n">
-        <f aca="false">C29/C$30*100</f>
+        <f aca="false">C29/C$31*100</f>
         <v>0</v>
       </c>
       <c r="M29" s="1" t="n">
-        <f aca="false">D29/D$30*100</f>
+        <f aca="false">D29/D$31*100</f>
         <v>0</v>
       </c>
       <c r="N29" s="1" t="n">
-        <f aca="false">E29/E$30*100</f>
+        <f aca="false">E29/E$31*100</f>
         <v>0</v>
       </c>
       <c r="O29" s="1" t="n">
-        <f aca="false">F29/F$30*100</f>
+        <f aca="false">F29/F$31*100</f>
         <v>0.00538806042546493</v>
       </c>
       <c r="P29" s="1" t="n">
-        <f aca="false">G29/G$30*100</f>
+        <f aca="false">G29/G$31*100</f>
         <v>0.00478957227697338</v>
       </c>
       <c r="Q29" s="1" t="n">
-        <f aca="false">H29/H$30*100</f>
+        <f aca="false">H29/H$31*100</f>
         <v>0</v>
       </c>
       <c r="R29" s="1" t="n">
-        <f aca="false">I29/I$30*100</f>
+        <f aca="false">I29/I$31*100</f>
         <v>0</v>
       </c>
     </row>
@@ -2061,67 +2086,104 @@
         <v>38</v>
       </c>
       <c r="B30" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C30" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" s="1" t="n">
+        <v>79200</v>
+      </c>
+      <c r="E30" s="1" t="n">
+        <v>8800</v>
+      </c>
+      <c r="F30" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I30" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="1"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="1" t="n">
         <f aca="false">SUM(B2:B23)</f>
         <v>661923490</v>
       </c>
-      <c r="C30" s="1" t="n">
+      <c r="C31" s="1" t="n">
         <f aca="false">SUM(C2:C23)</f>
         <v>82726741.6071429</v>
       </c>
-      <c r="D30" s="1" t="n">
+      <c r="D31" s="1" t="n">
         <f aca="false">SUM(D2:D23)</f>
         <v>933842400</v>
       </c>
-      <c r="E30" s="1" t="n">
+      <c r="E31" s="1" t="n">
         <f aca="false">SUM(E2:E23)</f>
         <v>116719173.214286</v>
       </c>
-      <c r="F30" s="1" t="n">
+      <c r="F31" s="1" t="n">
         <f aca="false">SUM(F2:F23)</f>
         <v>1469916700</v>
       </c>
-      <c r="G30" s="1" t="n">
+      <c r="G31" s="1" t="n">
         <f aca="false">SUM(G2:G23)</f>
         <v>183732481.547619</v>
       </c>
-      <c r="H30" s="1" t="n">
+      <c r="H31" s="1" t="n">
         <f aca="false">SUM(H2:H23)</f>
         <v>1736661300</v>
       </c>
-      <c r="I30" s="1" t="n">
+      <c r="I31" s="1" t="n">
         <f aca="false">SUM(I2:I23)</f>
         <v>217068016.071429</v>
       </c>
-      <c r="K30" s="1" t="n">
-        <f aca="false">B30/B$30*100</f>
+      <c r="K31" s="1" t="n">
+        <f aca="false">B31/B$31*100</f>
         <v>100</v>
       </c>
-      <c r="L30" s="1" t="n">
-        <f aca="false">C30/C$30*100</f>
+      <c r="L31" s="1" t="n">
+        <f aca="false">C31/C$31*100</f>
         <v>100</v>
       </c>
-      <c r="M30" s="1" t="n">
-        <f aca="false">D30/D$30*100</f>
+      <c r="M31" s="1" t="n">
+        <f aca="false">D31/D$31*100</f>
         <v>100</v>
       </c>
-      <c r="N30" s="1" t="n">
-        <f aca="false">E30/E$30*100</f>
+      <c r="N31" s="1" t="n">
+        <f aca="false">E31/E$31*100</f>
         <v>100</v>
       </c>
-      <c r="O30" s="1" t="n">
-        <f aca="false">F30/F$30*100</f>
+      <c r="O31" s="1" t="n">
+        <f aca="false">F31/F$31*100</f>
         <v>100</v>
       </c>
-      <c r="P30" s="1" t="n">
-        <f aca="false">G30/G$30*100</f>
+      <c r="P31" s="1" t="n">
+        <f aca="false">G31/G$31*100</f>
         <v>100</v>
       </c>
-      <c r="Q30" s="1" t="n">
-        <f aca="false">H30/H$30*100</f>
+      <c r="Q31" s="1" t="n">
+        <f aca="false">H31/H$31*100</f>
         <v>100</v>
       </c>
-      <c r="R30" s="1" t="n">
-        <f aca="false">I30/I$30*100</f>
+      <c r="R31" s="1" t="n">
+        <f aca="false">I31/I$31*100</f>
         <v>100</v>
       </c>
     </row>
@@ -2155,7 +2217,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>40</v>
@@ -2164,7 +2226,7 @@
         <v>41</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>40</v>
@@ -2753,7 +2815,7 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2765,7 +2827,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>40</v>
@@ -2774,7 +2836,7 @@
         <v>41</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>40</v>
@@ -2807,7 +2869,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>79200</v>
@@ -2816,7 +2878,7 @@
         <v>8800</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E3" s="0" t="n">
         <f aca="false">B3</f>
@@ -3357,7 +3419,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>40</v>
@@ -3366,7 +3428,7 @@
         <v>41</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>40</v>
@@ -3584,7 +3646,7 @@
         <v>6325000</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E11" s="1" t="n">
         <f aca="false">SUM(B31:B32)</f>
@@ -3606,7 +3668,7 @@
         <v>8800</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E12" s="0" t="n">
         <f aca="false">B33</f>
@@ -3628,7 +3690,7 @@
         <v>211250</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E13" s="0" t="n">
         <f aca="false">B34</f>
@@ -3894,7 +3956,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B31" s="1" t="n">
         <v>79200</v>
@@ -3905,7 +3967,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B32" s="1" t="n">
         <v>79200</v>
@@ -3916,7 +3978,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B33" s="1" t="n">
         <v>79200</v>
@@ -3927,7 +3989,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B34" s="1" t="n">
         <v>30400</v>
@@ -4234,7 +4296,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>40</v>
@@ -4243,7 +4305,7 @@
         <v>41</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>40</v>
@@ -4785,17 +4847,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F32" activeCellId="0" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>39</v>
+      <c r="A1" s="0" t="s">
+        <v>45</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>46</v>
@@ -4811,151 +4873,1286 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+      <c r="A2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>17.5151813995905</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>27.6059429299848</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>14.6224340467729</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>17.2971897283598</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
+      <c r="A3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>81.7167388937957</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>72.1122857561404</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>85.3001602063573</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>82.6126833136663</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="A4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>0.013838457372166</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>0.055148491865437</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>0.005388060425465</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="A5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>0.050051101827494</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>0.025443265373258</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>0.01077612085093</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>0.013681424236263</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+      <c r="A6" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>0.01196512908161</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>0.008481088457753</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>0.005388060425465</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+      <c r="A7" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>0.01196512908161</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>0.005388060425465</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="A8" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>0.088237586984699</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>0.062764109501375</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="A9" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>0.023930258163221</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>0.016164181276395</v>
+      </c>
+      <c r="E9" s="1" t="n">
+        <v>0.004560474745421</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>0.102610046366537</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>0.005388060425465</v>
+      </c>
+      <c r="E10" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="A11" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="A12" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+      <c r="A13" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="A14" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+      <c r="A15" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
+      <c r="A16" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>0.005388060425465</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="A17" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+      <c r="A18" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+      <c r="A19" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>0.008481088457753</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
+      <c r="A20" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <v>0.005388060425465</v>
+      </c>
+      <c r="E20" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
+      <c r="A21" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
+      <c r="A22" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="1" t="n">
+        <v>0.035895387244831</v>
+      </c>
+      <c r="C23" s="1" t="n">
+        <v>0.015088199036583</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1" t="n">
+        <v>0.004560474745421</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="1" t="n">
+        <v>0.01196512908161</v>
+      </c>
+      <c r="C24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1" t="n">
+        <v>0.001265377827193</v>
+      </c>
+      <c r="E24" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C25" s="1" t="n">
+        <v>0.008481088457753</v>
+      </c>
+      <c r="D25" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C26" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C27" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>0.005388060425465</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" s="1" t="n">
+        <v>0.035895387244831</v>
+      </c>
+      <c r="C29" s="1" t="n">
+        <v>0.012421796226001</v>
+      </c>
+      <c r="D29" s="1" t="n">
+        <v>0.02254549526514</v>
+      </c>
+      <c r="E29" s="1" t="n">
+        <v>0.004560474745421</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C30" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <v>0.04203467884037</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C33" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="1" t="n">
+        <v>0.481928810231527</v>
+      </c>
+      <c r="C34" s="1" t="n">
+        <v>0.068469797473321</v>
+      </c>
+      <c r="D34" s="1" t="n">
+        <v>0.005102329948357</v>
+      </c>
+      <c r="E34" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C36" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B37" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C37" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D37" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>0.01196512908161</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E37"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>17.5151813995905</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>27.6059429299848</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>14.6224340467729</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>17.2971897283598</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>81.7167388937957</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>72.1122857561404</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>85.3001602063573</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>82.6126833136663</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>0.013838457372166</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>0.055148491865437</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>0.005388060425465</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>0.050051101827494</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>0.025443265373258</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>0.01077612085093</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>0.013681424236263</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>0.01196512908161</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>0.008481088457753</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>0.005388060425465</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>0.01196512908161</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>0.005388060425465</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>0.088237586984699</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>0.062764109501375</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>0.023930258163221</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>0.016164181276395</v>
+      </c>
+      <c r="E9" s="1" t="n">
+        <v>0.004560474745421</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>0.102610046366537</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>0.005388060425465</v>
+      </c>
+      <c r="E10" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>0.005388060425465</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>0.008481088457753</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <v>0.005388060425465</v>
+      </c>
+      <c r="E20" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="1" t="n">
+        <v>0.035895387244831</v>
+      </c>
+      <c r="C23" s="1" t="n">
+        <v>0.015088199036583</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1" t="n">
+        <v>0.004560474745421</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="1" t="n">
+        <v>0.01196512908161</v>
+      </c>
+      <c r="C24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1" t="n">
+        <v>0.001265377827193</v>
+      </c>
+      <c r="E24" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C25" s="1" t="n">
+        <v>0.008481088457753</v>
+      </c>
+      <c r="D25" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C26" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C27" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>0.005388060425465</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" s="1" t="n">
+        <v>0.035895387244831</v>
+      </c>
+      <c r="C29" s="1" t="n">
+        <v>0.012421796226001</v>
+      </c>
+      <c r="D29" s="1" t="n">
+        <v>0.02254549526514</v>
+      </c>
+      <c r="E29" s="1" t="n">
+        <v>0.004560474745421</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C30" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <v>0.04203467884037</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C32" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33" s="1" t="n">
+        <v>0.481928810231527</v>
+      </c>
+      <c r="C33" s="1" t="n">
+        <v>0.068469797473321</v>
+      </c>
+      <c r="D33" s="1" t="n">
+        <v>0.005102329948357</v>
+      </c>
+      <c r="E33" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C34" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B36" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C36" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>0.01196512908161</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>